<commit_message>
output from ML approaches used
</commit_message>
<xml_diff>
--- a/output_files/outcome_machine_learning_for_acr_values.xlsx
+++ b/output_files/outcome_machine_learning_for_acr_values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="525" windowWidth="8295" windowHeight="5835"/>
+    <workbookView xWindow="270" yWindow="525" windowWidth="8295" windowHeight="5835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="raw output" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
   <si>
     <t>Feature Data</t>
   </si>
@@ -133,7 +133,10 @@
     <t>6927, 87:[6032,0,895,0]</t>
   </si>
   <si>
-    <t>Abs() : Accuracy/performance: Test R2 Score</t>
+    <t>Abs:Accuracy/performance</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -203,6 +206,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -234,7 +258,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -286,8 +310,32 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -589,25 +637,24 @@
   </sheetPr>
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="115.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="112.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
@@ -816,7 +863,7 @@
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="9"/>
@@ -843,7 +890,7 @@
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="9"/>
@@ -870,7 +917,7 @@
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="9"/>
@@ -1146,57 +1193,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="115.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15.75" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="23" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="11" t="s">
@@ -1231,24 +1278,24 @@
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
       <c r="A2" s="6">
-        <f>ABS(J2)</f>
+        <f t="shared" ref="A2:A16" si="0">ABS(J2)</f>
         <v>0.95656716873844105</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="7">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="19">
         <v>-0.95656716873844105</v>
       </c>
       <c r="K2" s="7"/>
@@ -1262,24 +1309,24 @@
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
       <c r="A3" s="6">
-        <f>ABS(J3)</f>
+        <f t="shared" si="0"/>
         <v>0.68159765149028495</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="B3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="7">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="19">
         <v>-0.68159765149028495</v>
       </c>
       <c r="K3" s="7"/>
@@ -1293,34 +1340,34 @@
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
       <c r="A4" s="6">
-        <f>ABS(J4)</f>
+        <f t="shared" si="0"/>
         <v>0.57871423499755503</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="26">
         <v>90965</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="27">
         <v>52946.429645249002</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="28">
         <v>301.60419042591201</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="29">
         <v>301.60419042591201</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="19">
         <v>0.35873042074282802</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="20">
         <v>-0.57871423499755503</v>
       </c>
       <c r="K4" s="8"/>
@@ -1329,34 +1376,34 @@
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
       <c r="A5" s="6">
-        <f>ABS(J5)</f>
+        <f t="shared" si="0"/>
         <v>0.41427970553851001</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="31">
         <v>93047.912073294297</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="20">
         <v>47431.675263328601</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="19">
         <v>305.03755846336998</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="20">
         <v>305.03755846336998</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="19">
         <v>0.34404729389934302</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="20">
         <v>-0.41427970553851001</v>
       </c>
       <c r="K5" s="8"/>
@@ -1365,24 +1412,24 @@
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
       <c r="A6" s="6">
-        <f>ABS(J6)</f>
+        <f t="shared" si="0"/>
         <v>0.39438000000000001</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="B6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="7">
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="19">
         <v>-0.39438000000000001</v>
       </c>
       <c r="K6" s="7"/>
@@ -1396,24 +1443,24 @@
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
       <c r="A7" s="6">
-        <f>ABS(J7)</f>
+        <f t="shared" si="0"/>
         <v>0.134377214453441</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="7">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="19">
         <v>-0.134377214453441</v>
       </c>
       <c r="K7" s="7"/>
@@ -1427,24 +1474,24 @@
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
       <c r="A8" s="6">
-        <f>ABS(J8)</f>
+        <f t="shared" si="0"/>
         <v>0.134377214453441</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="7">
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="19">
         <v>-0.134377214453441</v>
       </c>
       <c r="K8" s="7"/>
@@ -1458,34 +1505,34 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
       <c r="A9" s="6">
-        <f>ABS(J9)</f>
+        <f t="shared" si="0"/>
         <v>7.7241555975166895E-2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="31">
         <v>139019.96385302101</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="20">
         <v>36128.194064498297</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="19">
         <v>372.85381029704001</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="20">
         <v>190.074180425691</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="19">
         <v>1.9961657822329101E-2</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="20">
         <v>-7.7241555975166895E-2</v>
       </c>
       <c r="K9" s="8"/>
@@ -1494,34 +1541,34 @@
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
       <c r="A10" s="6">
-        <f>ABS(J10)</f>
+        <f t="shared" si="0"/>
         <v>7.7241555975166895E-2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="B10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="31">
         <v>139019.96385302101</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="20">
         <v>36128.194064498297</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="19">
         <v>372.85381029704001</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="20">
         <v>190.074180425691</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="19">
         <v>1.99616578223289E-2</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="20">
         <v>-7.7241555975166895E-2</v>
       </c>
       <c r="K10" s="8"/>
@@ -1530,34 +1577,34 @@
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1">
       <c r="A11" s="6">
-        <f>ABS(J11)</f>
+        <f t="shared" si="0"/>
         <v>5.6434307242474599E-2</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="31">
         <v>139091.64835314301</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="20">
         <v>35430.366993129501</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="19">
         <v>372.94992740734398</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="20">
         <v>372.94992740734398</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="19">
         <v>1.9456309117636902E-2</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="20">
         <v>-5.6434307242474599E-2</v>
       </c>
       <c r="K11" s="8"/>
@@ -1566,24 +1613,24 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
       <c r="A12" s="6">
-        <f>ABS(J12)</f>
+        <f t="shared" si="0"/>
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="7">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="19">
         <v>-5.2999999999999999E-2</v>
       </c>
       <c r="K12" s="7"/>
@@ -1597,21 +1644,22 @@
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
       <c r="A13" s="6">
-        <f>ABS(J13)</f>
+        <f t="shared" si="0"/>
         <v>5.2499999999999998E-2</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="7">
+      <c r="D13" s="12"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="19">
         <v>-5.2499999999999998E-2</v>
       </c>
       <c r="K13" s="7"/>
@@ -1625,34 +1673,34 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
       <c r="A14" s="6">
-        <f>ABS(J14)</f>
+        <f t="shared" si="0"/>
         <v>2.4E-2</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="31">
         <v>77719.25</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="20">
         <v>34344.339999999997</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="19">
         <v>278.77999999999997</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="20">
         <v>278.77999999999997</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="19">
         <v>0.45200000000000001</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="20">
         <v>-2.4E-2</v>
       </c>
       <c r="K14" s="8"/>
@@ -1661,34 +1709,34 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1">
       <c r="A15" s="6">
-        <f>ABS(J15)</f>
+        <f t="shared" si="0"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="26">
         <v>0.112</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="29">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="19">
         <v>0.33500000000000002</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="20">
         <v>0.30299999999999999</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="28">
         <v>5.2077511719068603E-3</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="29">
         <v>-8.0000000000000002E-3</v>
       </c>
       <c r="K15" s="17" t="s">
@@ -1701,34 +1749,34 @@
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1">
       <c r="A16" s="6">
-        <f>ABS(J16)</f>
+        <f t="shared" si="0"/>
         <v>2.8E-3</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="31">
         <v>0.11193</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="20">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="19">
         <v>0.33500000000000002</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="20">
         <v>0.30299999999999999</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="19">
         <v>5.2077511719068603E-3</v>
       </c>
-      <c r="J16" s="8">
+      <c r="J16" s="20">
         <v>-2.8E-3</v>
       </c>
       <c r="K16" s="17" t="s">

</xml_diff>